<commit_message>
Small updates to make sure whole script runs smoothly
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_220401.xlsx
+++ b/data/hake_intrasp_220401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F14C8F-2877-8C42-A3BD-8D846D5AE113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D842CE26-94C3-7B49-B0CC-1360ED1225FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="38400" windowHeight="42700" firstSheet="3" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -14957,7 +14957,7 @@
   <dimension ref="A1:AG42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="R81" sqref="R81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18106,8 +18106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView zoomScale="175" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18288,8 +18288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:I401"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E122" sqref="E122:E141"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O105" sqref="O105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29936,7 +29936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:I401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+    <sheetView topLeftCell="A94" workbookViewId="0">
       <selection activeCell="R142" sqref="R142"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Continuing to try to get the predation models to work. Bleh.
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_220401.xlsx
+++ b/data/hake_intrasp_220401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CC624A-8C0F-4E49-9AD4-B4798477C584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F2ADC9-9B15-D641-9D89-743FA69C9714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="33340" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="33340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">UobsWtAge!$A$1:$I$221</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1962,7 +1974,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14494,8 +14506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14545,7 +14557,7 @@
         <v>144</v>
       </c>
       <c r="B6">
-        <v>0.16700000000000001</v>
+        <v>8.3500000000000005E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -14954,10 +14966,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:AG42"/>
+  <dimension ref="A1:AG41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R81" sqref="R81"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15071,7 +15083,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1979</v>
+        <v>1980</v>
       </c>
       <c r="D2">
         <v>126.1455</v>
@@ -15145,70 +15157,70 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1980</v>
+        <v>1981</v>
       </c>
       <c r="D3">
-        <v>126.1455</v>
+        <v>98.492800000000003</v>
       </c>
       <c r="E3">
-        <v>125.4808</v>
+        <v>96.543199999999999</v>
       </c>
       <c r="F3">
-        <v>124.1448</v>
+        <v>92.692999999999998</v>
       </c>
       <c r="G3">
-        <v>122.24339999999999</v>
+        <v>87.265799999999999</v>
       </c>
       <c r="H3">
-        <v>118.321</v>
+        <v>79.953199999999995</v>
       </c>
       <c r="I3">
-        <v>111.29989999999999</v>
+        <v>71.131600000000006</v>
       </c>
       <c r="J3">
-        <v>107.32980000000001</v>
+        <v>65.597899999999996</v>
       </c>
       <c r="K3">
-        <v>106.9545</v>
+        <v>63.941299999999998</v>
       </c>
       <c r="L3">
-        <v>110.6833</v>
+        <v>66.706100000000006</v>
       </c>
       <c r="M3">
-        <v>118.85590000000001</v>
+        <v>74.498500000000007</v>
       </c>
       <c r="N3">
-        <v>131.4879</v>
+        <v>87.907899999999998</v>
       </c>
       <c r="O3">
-        <v>148.04499999999999</v>
+        <v>107.06229999999999</v>
       </c>
       <c r="P3">
-        <v>167.22630000000001</v>
+        <v>130.85820000000001</v>
       </c>
       <c r="Q3">
-        <v>186.94229999999999</v>
+        <v>156.3057</v>
       </c>
       <c r="R3">
-        <v>204.64439999999999</v>
+        <v>178.74529999999999</v>
       </c>
       <c r="S3">
-        <v>217.95769999999999</v>
+        <v>193.3117</v>
       </c>
       <c r="T3">
-        <v>225.3289</v>
+        <v>196.9417</v>
       </c>
       <c r="U3">
-        <v>226.36619999999999</v>
+        <v>189.5521</v>
       </c>
       <c r="V3">
-        <v>221.74359999999999</v>
+        <v>173.65899999999999</v>
       </c>
       <c r="W3">
-        <v>212.80459999999999</v>
+        <v>152.9573</v>
       </c>
       <c r="X3">
-        <v>201.0616</v>
+        <v>130.83930000000001</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
@@ -15219,70 +15231,70 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1981</v>
+        <v>1982</v>
       </c>
       <c r="D4">
-        <v>98.492800000000003</v>
+        <v>174.9512</v>
       </c>
       <c r="E4">
-        <v>96.543199999999999</v>
+        <v>174.76609999999999</v>
       </c>
       <c r="F4">
-        <v>92.692999999999998</v>
+        <v>174.40129999999999</v>
       </c>
       <c r="G4">
-        <v>87.265799999999999</v>
+        <v>173.9589</v>
       </c>
       <c r="H4">
-        <v>79.953199999999995</v>
+        <v>171.0532</v>
       </c>
       <c r="I4">
-        <v>71.131600000000006</v>
+        <v>163.49950000000001</v>
       </c>
       <c r="J4">
-        <v>65.597899999999996</v>
+        <v>159.703</v>
       </c>
       <c r="K4">
-        <v>63.941299999999998</v>
+        <v>160.1568</v>
       </c>
       <c r="L4">
-        <v>66.706100000000006</v>
+        <v>165.3571</v>
       </c>
       <c r="M4">
-        <v>74.498500000000007</v>
+        <v>175.57669999999999</v>
       </c>
       <c r="N4">
-        <v>87.907899999999998</v>
+        <v>190.67150000000001</v>
       </c>
       <c r="O4">
-        <v>107.06229999999999</v>
+        <v>209.89400000000001</v>
       </c>
       <c r="P4">
-        <v>130.85820000000001</v>
+        <v>231.77860000000001</v>
       </c>
       <c r="Q4">
-        <v>156.3057</v>
+        <v>254.22190000000001</v>
       </c>
       <c r="R4">
-        <v>178.74529999999999</v>
+        <v>274.8261</v>
       </c>
       <c r="S4">
-        <v>193.3117</v>
+        <v>291.42039999999997</v>
       </c>
       <c r="T4">
-        <v>196.9417</v>
+        <v>302.54700000000003</v>
       </c>
       <c r="U4">
-        <v>189.5521</v>
+        <v>307.70209999999997</v>
       </c>
       <c r="V4">
-        <v>173.65899999999999</v>
+        <v>307.26929999999999</v>
       </c>
       <c r="W4">
-        <v>152.9573</v>
+        <v>302.23809999999997</v>
       </c>
       <c r="X4">
-        <v>130.83930000000001</v>
+        <v>293.83179999999999</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -15293,70 +15305,70 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>1982</v>
+        <v>1983</v>
       </c>
       <c r="D5">
-        <v>174.9512</v>
+        <v>124.96550000000001</v>
       </c>
       <c r="E5">
-        <v>174.76609999999999</v>
+        <v>123.24299999999999</v>
       </c>
       <c r="F5">
-        <v>174.40129999999999</v>
+        <v>119.8253</v>
       </c>
       <c r="G5">
-        <v>173.9589</v>
+        <v>114.9632</v>
       </c>
       <c r="H5">
-        <v>171.0532</v>
+        <v>107.93519999999999</v>
       </c>
       <c r="I5">
-        <v>163.49950000000001</v>
+        <v>98.287099999999995</v>
       </c>
       <c r="J5">
-        <v>159.703</v>
+        <v>92.247900000000001</v>
       </c>
       <c r="K5">
-        <v>160.1568</v>
+        <v>90.502700000000004</v>
       </c>
       <c r="L5">
-        <v>165.3571</v>
+        <v>93.665000000000006</v>
       </c>
       <c r="M5">
-        <v>175.57669999999999</v>
+        <v>102.2809</v>
       </c>
       <c r="N5">
-        <v>190.67150000000001</v>
+        <v>116.71720000000001</v>
       </c>
       <c r="O5">
-        <v>209.89400000000001</v>
+        <v>136.80109999999999</v>
       </c>
       <c r="P5">
-        <v>231.77860000000001</v>
+        <v>161.2852</v>
       </c>
       <c r="Q5">
-        <v>254.22190000000001</v>
+        <v>187.47559999999999</v>
       </c>
       <c r="R5">
-        <v>274.8261</v>
+        <v>211.48089999999999</v>
       </c>
       <c r="S5">
-        <v>291.42039999999997</v>
+        <v>229.24029999999999</v>
       </c>
       <c r="T5">
-        <v>302.54700000000003</v>
+        <v>237.88409999999999</v>
       </c>
       <c r="U5">
-        <v>307.70209999999997</v>
+        <v>236.62710000000001</v>
       </c>
       <c r="V5">
-        <v>307.26929999999999</v>
+        <v>226.72550000000001</v>
       </c>
       <c r="W5">
-        <v>302.23809999999997</v>
+        <v>210.6893</v>
       </c>
       <c r="X5">
-        <v>293.83179999999999</v>
+        <v>191.25540000000001</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
@@ -15367,70 +15379,70 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="D6">
-        <v>124.96550000000001</v>
+        <v>88.7196</v>
       </c>
       <c r="E6">
-        <v>123.24299999999999</v>
+        <v>87.267300000000006</v>
       </c>
       <c r="F6">
-        <v>119.8253</v>
+        <v>84.417199999999994</v>
       </c>
       <c r="G6">
-        <v>114.9632</v>
+        <v>80.396199999999993</v>
       </c>
       <c r="H6">
-        <v>107.93519999999999</v>
+        <v>74.997399999999999</v>
       </c>
       <c r="I6">
-        <v>98.287099999999995</v>
+        <v>67.644199999999998</v>
       </c>
       <c r="J6">
-        <v>92.247900000000001</v>
+        <v>62.863999999999997</v>
       </c>
       <c r="K6">
-        <v>90.502700000000004</v>
+        <v>61.093000000000004</v>
       </c>
       <c r="L6">
-        <v>93.665000000000006</v>
+        <v>62.705599999999997</v>
       </c>
       <c r="M6">
-        <v>102.2809</v>
+        <v>68.052400000000006</v>
       </c>
       <c r="N6">
-        <v>116.71720000000001</v>
+        <v>77.424400000000006</v>
       </c>
       <c r="O6">
-        <v>136.80109999999999</v>
+        <v>90.849500000000006</v>
       </c>
       <c r="P6">
-        <v>161.2852</v>
+        <v>107.7466</v>
       </c>
       <c r="Q6">
-        <v>187.47559999999999</v>
+        <v>126.6161</v>
       </c>
       <c r="R6">
-        <v>211.48089999999999</v>
+        <v>145.05760000000001</v>
       </c>
       <c r="S6">
-        <v>229.24029999999999</v>
+        <v>160.2869</v>
       </c>
       <c r="T6">
-        <v>237.88409999999999</v>
+        <v>169.98570000000001</v>
       </c>
       <c r="U6">
-        <v>236.62710000000001</v>
+        <v>173.0223</v>
       </c>
       <c r="V6">
-        <v>226.72550000000001</v>
+        <v>169.65389999999999</v>
       </c>
       <c r="W6">
-        <v>210.6893</v>
+        <v>161.19159999999999</v>
       </c>
       <c r="X6">
-        <v>191.25540000000001</v>
+        <v>149.37389999999999</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
@@ -15441,70 +15453,70 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="D7">
-        <v>88.7196</v>
+        <v>135.7364</v>
       </c>
       <c r="E7">
-        <v>87.267300000000006</v>
+        <v>134.64080000000001</v>
       </c>
       <c r="F7">
-        <v>84.417199999999994</v>
+        <v>132.44309999999999</v>
       </c>
       <c r="G7">
-        <v>80.396199999999993</v>
+        <v>129.2962</v>
       </c>
       <c r="H7">
-        <v>74.997399999999999</v>
+        <v>123.8343</v>
       </c>
       <c r="I7">
-        <v>67.644199999999998</v>
+        <v>115.24760000000001</v>
       </c>
       <c r="J7">
-        <v>62.863999999999997</v>
+        <v>110.18989999999999</v>
       </c>
       <c r="K7">
-        <v>61.093000000000004</v>
+        <v>109.3439</v>
       </c>
       <c r="L7">
-        <v>62.705599999999997</v>
+        <v>113.3366</v>
       </c>
       <c r="M7">
-        <v>68.052400000000006</v>
+        <v>122.6326</v>
       </c>
       <c r="N7">
-        <v>77.424400000000006</v>
+        <v>137.36429999999999</v>
       </c>
       <c r="O7">
-        <v>90.849500000000006</v>
+        <v>157.01750000000001</v>
       </c>
       <c r="P7">
-        <v>107.7466</v>
+        <v>180.07079999999999</v>
       </c>
       <c r="Q7">
-        <v>126.6161</v>
+        <v>203.875</v>
       </c>
       <c r="R7">
-        <v>145.05760000000001</v>
+        <v>225.04810000000001</v>
       </c>
       <c r="S7">
-        <v>160.2869</v>
+        <v>240.37360000000001</v>
       </c>
       <c r="T7">
-        <v>169.98570000000001</v>
+        <v>247.7756</v>
       </c>
       <c r="U7">
-        <v>173.0223</v>
+        <v>246.8432</v>
       </c>
       <c r="V7">
-        <v>169.65389999999999</v>
+        <v>238.67850000000001</v>
       </c>
       <c r="W7">
-        <v>161.19159999999999</v>
+        <v>225.27979999999999</v>
       </c>
       <c r="X7">
-        <v>149.37389999999999</v>
+        <v>208.79150000000001</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.2">
@@ -15515,70 +15527,70 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="D8">
-        <v>135.7364</v>
+        <v>141.94730000000001</v>
       </c>
       <c r="E8">
-        <v>134.64080000000001</v>
+        <v>141.9066</v>
       </c>
       <c r="F8">
-        <v>132.44309999999999</v>
+        <v>141.83349999999999</v>
       </c>
       <c r="G8">
-        <v>129.2962</v>
+        <v>141.80719999999999</v>
       </c>
       <c r="H8">
-        <v>123.8343</v>
+        <v>139.8681</v>
       </c>
       <c r="I8">
-        <v>115.24760000000001</v>
+        <v>134.08090000000001</v>
       </c>
       <c r="J8">
-        <v>110.18989999999999</v>
+        <v>131.26060000000001</v>
       </c>
       <c r="K8">
-        <v>109.3439</v>
+        <v>131.7543</v>
       </c>
       <c r="L8">
-        <v>113.3366</v>
+        <v>135.92189999999999</v>
       </c>
       <c r="M8">
-        <v>122.6326</v>
+        <v>143.952</v>
       </c>
       <c r="N8">
-        <v>137.36429999999999</v>
+        <v>155.7124</v>
       </c>
       <c r="O8">
-        <v>157.01750000000001</v>
+        <v>170.6183</v>
       </c>
       <c r="P8">
-        <v>180.07079999999999</v>
+        <v>187.56139999999999</v>
       </c>
       <c r="Q8">
-        <v>203.875</v>
+        <v>204.98140000000001</v>
       </c>
       <c r="R8">
-        <v>225.04810000000001</v>
+        <v>221.11689999999999</v>
       </c>
       <c r="S8">
-        <v>240.37360000000001</v>
+        <v>234.3751</v>
       </c>
       <c r="T8">
-        <v>247.7756</v>
+        <v>243.66829999999999</v>
       </c>
       <c r="U8">
-        <v>246.8432</v>
+        <v>248.58529999999999</v>
       </c>
       <c r="V8">
-        <v>238.67850000000001</v>
+        <v>249.34870000000001</v>
       </c>
       <c r="W8">
-        <v>225.27979999999999</v>
+        <v>246.62549999999999</v>
       </c>
       <c r="X8">
-        <v>208.79150000000001</v>
+        <v>241.27199999999999</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.2">
@@ -15589,70 +15601,70 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="D9">
-        <v>141.94730000000001</v>
+        <v>106.0604</v>
       </c>
       <c r="E9">
-        <v>141.9066</v>
+        <v>104.5821</v>
       </c>
       <c r="F9">
-        <v>141.83349999999999</v>
+        <v>101.6985</v>
       </c>
       <c r="G9">
-        <v>141.80719999999999</v>
+        <v>97.634</v>
       </c>
       <c r="H9">
-        <v>139.8681</v>
+        <v>92.279899999999998</v>
       </c>
       <c r="I9">
-        <v>134.08090000000001</v>
+        <v>84.043700000000001</v>
       </c>
       <c r="J9">
-        <v>131.26060000000001</v>
+        <v>78.553799999999995</v>
       </c>
       <c r="K9">
-        <v>131.7543</v>
+        <v>76.236999999999995</v>
       </c>
       <c r="L9">
-        <v>135.92189999999999</v>
+        <v>77.447000000000003</v>
       </c>
       <c r="M9">
-        <v>143.952</v>
+        <v>82.471999999999994</v>
       </c>
       <c r="N9">
-        <v>155.7124</v>
+        <v>91.508099999999999</v>
       </c>
       <c r="O9">
-        <v>170.6183</v>
+        <v>104.524</v>
       </c>
       <c r="P9">
-        <v>187.56139999999999</v>
+        <v>121.03230000000001</v>
       </c>
       <c r="Q9">
-        <v>204.98140000000001</v>
+        <v>139.88489999999999</v>
       </c>
       <c r="R9">
-        <v>221.11689999999999</v>
+        <v>159.26179999999999</v>
       </c>
       <c r="S9">
-        <v>234.3751</v>
+        <v>176.9641</v>
       </c>
       <c r="T9">
-        <v>243.66829999999999</v>
+        <v>190.93899999999999</v>
       </c>
       <c r="U9">
-        <v>248.58529999999999</v>
+        <v>199.79990000000001</v>
       </c>
       <c r="V9">
-        <v>249.34870000000001</v>
+        <v>203.09809999999999</v>
       </c>
       <c r="W9">
-        <v>246.62549999999999</v>
+        <v>201.26410000000001</v>
       </c>
       <c r="X9">
-        <v>241.27199999999999</v>
+        <v>195.29329999999999</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.2">
@@ -15663,70 +15675,70 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="D10">
-        <v>106.0604</v>
+        <v>119.8438</v>
       </c>
       <c r="E10">
-        <v>104.5821</v>
+        <v>119.6365</v>
       </c>
       <c r="F10">
-        <v>101.6985</v>
+        <v>119.2217</v>
       </c>
       <c r="G10">
-        <v>97.634</v>
+        <v>118.6739</v>
       </c>
       <c r="H10">
-        <v>92.279899999999998</v>
+        <v>116.2269</v>
       </c>
       <c r="I10">
-        <v>84.043700000000001</v>
+        <v>110.8245</v>
       </c>
       <c r="J10">
-        <v>78.553799999999995</v>
+        <v>108.1249</v>
       </c>
       <c r="K10">
-        <v>76.236999999999995</v>
+        <v>108.538</v>
       </c>
       <c r="L10">
-        <v>77.447000000000003</v>
+        <v>112.4649</v>
       </c>
       <c r="M10">
-        <v>82.471999999999994</v>
+        <v>120.1336</v>
       </c>
       <c r="N10">
-        <v>91.508099999999999</v>
+        <v>131.44380000000001</v>
       </c>
       <c r="O10">
-        <v>104.524</v>
+        <v>145.80179999999999</v>
       </c>
       <c r="P10">
-        <v>121.03230000000001</v>
+        <v>162.0103</v>
       </c>
       <c r="Q10">
-        <v>139.88489999999999</v>
+        <v>178.33459999999999</v>
       </c>
       <c r="R10">
-        <v>159.26179999999999</v>
+        <v>192.81229999999999</v>
       </c>
       <c r="S10">
-        <v>176.9641</v>
+        <v>203.72540000000001</v>
       </c>
       <c r="T10">
-        <v>190.93899999999999</v>
+        <v>210.0222</v>
       </c>
       <c r="U10">
-        <v>199.79990000000001</v>
+        <v>211.49510000000001</v>
       </c>
       <c r="V10">
-        <v>203.09809999999999</v>
+        <v>208.67240000000001</v>
       </c>
       <c r="W10">
-        <v>201.26410000000001</v>
+        <v>202.52959999999999</v>
       </c>
       <c r="X10">
-        <v>195.29329999999999</v>
+        <v>194.1514</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.2">
@@ -15737,70 +15749,70 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="D11">
-        <v>119.8438</v>
+        <v>124.4431</v>
       </c>
       <c r="E11">
-        <v>119.6365</v>
+        <v>122.929</v>
       </c>
       <c r="F11">
-        <v>119.2217</v>
+        <v>119.92529999999999</v>
       </c>
       <c r="G11">
-        <v>118.6739</v>
+        <v>115.6474</v>
       </c>
       <c r="H11">
-        <v>116.2269</v>
+        <v>109.3439</v>
       </c>
       <c r="I11">
-        <v>110.8245</v>
+        <v>100.1932</v>
       </c>
       <c r="J11">
-        <v>108.1249</v>
+        <v>94.456900000000005</v>
       </c>
       <c r="K11">
-        <v>108.538</v>
+        <v>92.7714</v>
       </c>
       <c r="L11">
-        <v>112.4649</v>
+        <v>95.703400000000002</v>
       </c>
       <c r="M11">
-        <v>120.1336</v>
+        <v>103.7265</v>
       </c>
       <c r="N11">
-        <v>131.44380000000001</v>
+        <v>117.11620000000001</v>
       </c>
       <c r="O11">
-        <v>145.80179999999999</v>
+        <v>135.65539999999999</v>
       </c>
       <c r="P11">
-        <v>162.0103</v>
+        <v>158.2165</v>
       </c>
       <c r="Q11">
-        <v>178.33459999999999</v>
+        <v>182.4846</v>
       </c>
       <c r="R11">
-        <v>192.81229999999999</v>
+        <v>205.16650000000001</v>
       </c>
       <c r="S11">
-        <v>203.72540000000001</v>
+        <v>222.7938</v>
       </c>
       <c r="T11">
-        <v>210.0222</v>
+        <v>232.79169999999999</v>
       </c>
       <c r="U11">
-        <v>211.49510000000001</v>
+        <v>234.22040000000001</v>
       </c>
       <c r="V11">
-        <v>208.67240000000001</v>
+        <v>227.82560000000001</v>
       </c>
       <c r="W11">
-        <v>202.52959999999999</v>
+        <v>215.49170000000001</v>
       </c>
       <c r="X11">
-        <v>194.1514</v>
+        <v>199.44579999999999</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.2">
@@ -15811,70 +15823,70 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="D12">
-        <v>124.4431</v>
+        <v>120.8061</v>
       </c>
       <c r="E12">
-        <v>122.929</v>
+        <v>120.0605</v>
       </c>
       <c r="F12">
-        <v>119.92529999999999</v>
+        <v>118.5757</v>
       </c>
       <c r="G12">
-        <v>115.6474</v>
+        <v>116.4637</v>
       </c>
       <c r="H12">
-        <v>109.3439</v>
+        <v>112.71729999999999</v>
       </c>
       <c r="I12">
-        <v>100.1932</v>
+        <v>105.66419999999999</v>
       </c>
       <c r="J12">
-        <v>94.456900000000005</v>
+        <v>101.4285</v>
       </c>
       <c r="K12">
-        <v>92.7714</v>
+        <v>100.47280000000001</v>
       </c>
       <c r="L12">
-        <v>95.703400000000002</v>
+        <v>103.22450000000001</v>
       </c>
       <c r="M12">
-        <v>103.7265</v>
+        <v>109.9739</v>
       </c>
       <c r="N12">
-        <v>117.11620000000001</v>
+        <v>120.76730000000001</v>
       </c>
       <c r="O12">
-        <v>135.65539999999999</v>
+        <v>135.244</v>
       </c>
       <c r="P12">
-        <v>158.2165</v>
+        <v>152.46270000000001</v>
       </c>
       <c r="Q12">
-        <v>182.4846</v>
+        <v>170.84460000000001</v>
       </c>
       <c r="R12">
-        <v>205.16650000000001</v>
+        <v>188.35890000000001</v>
       </c>
       <c r="S12">
-        <v>222.7938</v>
+        <v>202.95179999999999</v>
       </c>
       <c r="T12">
-        <v>232.79169999999999</v>
+        <v>213.05080000000001</v>
       </c>
       <c r="U12">
-        <v>234.22040000000001</v>
+        <v>217.911</v>
       </c>
       <c r="V12">
-        <v>227.82560000000001</v>
+        <v>217.66370000000001</v>
       </c>
       <c r="W12">
-        <v>215.49170000000001</v>
+        <v>213.1063</v>
       </c>
       <c r="X12">
-        <v>199.44579999999999</v>
+        <v>205.34800000000001</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.2">
@@ -15885,70 +15897,70 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="D13">
-        <v>120.8061</v>
+        <v>118.37179999999999</v>
       </c>
       <c r="E13">
-        <v>120.0605</v>
+        <v>117.7453</v>
       </c>
       <c r="F13">
-        <v>118.5757</v>
+        <v>116.4927</v>
       </c>
       <c r="G13">
-        <v>116.4637</v>
+        <v>114.71339999999999</v>
       </c>
       <c r="H13">
-        <v>112.71729999999999</v>
+        <v>111.23569999999999</v>
       </c>
       <c r="I13">
-        <v>105.66419999999999</v>
+        <v>104.6224</v>
       </c>
       <c r="J13">
-        <v>101.4285</v>
+        <v>100.7739</v>
       </c>
       <c r="K13">
-        <v>100.47280000000001</v>
+        <v>100.1502</v>
       </c>
       <c r="L13">
-        <v>103.22450000000001</v>
+        <v>103.18170000000001</v>
       </c>
       <c r="M13">
-        <v>109.9739</v>
+        <v>110.15389999999999</v>
       </c>
       <c r="N13">
-        <v>120.76730000000001</v>
+        <v>121.0872</v>
       </c>
       <c r="O13">
-        <v>135.244</v>
+        <v>135.56540000000001</v>
       </c>
       <c r="P13">
-        <v>152.46270000000001</v>
+        <v>152.56710000000001</v>
       </c>
       <c r="Q13">
-        <v>170.84460000000001</v>
+        <v>170.4332</v>
       </c>
       <c r="R13">
-        <v>188.35890000000001</v>
+        <v>187.0916</v>
       </c>
       <c r="S13">
-        <v>202.95179999999999</v>
+        <v>200.52109999999999</v>
       </c>
       <c r="T13">
-        <v>213.05080000000001</v>
+        <v>209.261</v>
       </c>
       <c r="U13">
-        <v>217.911</v>
+        <v>212.72559999999999</v>
       </c>
       <c r="V13">
-        <v>217.66370000000001</v>
+        <v>211.20509999999999</v>
       </c>
       <c r="W13">
-        <v>213.1063</v>
+        <v>205.61179999999999</v>
       </c>
       <c r="X13">
-        <v>205.34800000000001</v>
+        <v>197.10740000000001</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.2">
@@ -15959,70 +15971,70 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="D14">
-        <v>118.37179999999999</v>
+        <v>129.21039999999999</v>
       </c>
       <c r="E14">
-        <v>117.7453</v>
+        <v>129.55359999999999</v>
       </c>
       <c r="F14">
-        <v>116.4927</v>
+        <v>130.26900000000001</v>
       </c>
       <c r="G14">
-        <v>114.71339999999999</v>
+        <v>131.4315</v>
       </c>
       <c r="H14">
-        <v>111.23569999999999</v>
+        <v>130.8347</v>
       </c>
       <c r="I14">
-        <v>104.6224</v>
+        <v>126.8557</v>
       </c>
       <c r="J14">
-        <v>100.7739</v>
+        <v>125.423</v>
       </c>
       <c r="K14">
-        <v>100.1502</v>
+        <v>126.70569999999999</v>
       </c>
       <c r="L14">
-        <v>103.18170000000001</v>
+        <v>130.91489999999999</v>
       </c>
       <c r="M14">
-        <v>110.15389999999999</v>
+        <v>138.1293</v>
       </c>
       <c r="N14">
-        <v>121.0872</v>
+        <v>148.16589999999999</v>
       </c>
       <c r="O14">
-        <v>135.56540000000001</v>
+        <v>160.4941</v>
       </c>
       <c r="P14">
-        <v>152.56710000000001</v>
+        <v>174.2218</v>
       </c>
       <c r="Q14">
-        <v>170.4332</v>
+        <v>188.1876</v>
       </c>
       <c r="R14">
-        <v>187.0916</v>
+        <v>201.15880000000001</v>
       </c>
       <c r="S14">
-        <v>200.52109999999999</v>
+        <v>212.0737</v>
       </c>
       <c r="T14">
-        <v>209.261</v>
+        <v>220.23650000000001</v>
       </c>
       <c r="U14">
-        <v>212.72559999999999</v>
+        <v>225.39660000000001</v>
       </c>
       <c r="V14">
-        <v>211.20509999999999</v>
+        <v>227.70179999999999</v>
       </c>
       <c r="W14">
-        <v>205.61179999999999</v>
+        <v>227.57300000000001</v>
       </c>
       <c r="X14">
-        <v>197.10740000000001</v>
+        <v>225.55250000000001</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.2">
@@ -16033,70 +16045,70 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="D15">
-        <v>129.21039999999999</v>
+        <v>119.36360000000001</v>
       </c>
       <c r="E15">
-        <v>129.55359999999999</v>
+        <v>118.12430000000001</v>
       </c>
       <c r="F15">
-        <v>130.26900000000001</v>
+        <v>115.6494</v>
       </c>
       <c r="G15">
-        <v>131.4315</v>
+        <v>112.1101</v>
       </c>
       <c r="H15">
-        <v>130.8347</v>
+        <v>106.51739999999999</v>
       </c>
       <c r="I15">
-        <v>126.8557</v>
+        <v>98.261499999999998</v>
       </c>
       <c r="J15">
-        <v>125.423</v>
+        <v>93.247200000000007</v>
       </c>
       <c r="K15">
-        <v>126.70569999999999</v>
+        <v>92.106499999999997</v>
       </c>
       <c r="L15">
-        <v>130.91489999999999</v>
+        <v>95.413200000000003</v>
       </c>
       <c r="M15">
-        <v>138.1293</v>
+        <v>103.626</v>
       </c>
       <c r="N15">
-        <v>148.16589999999999</v>
+        <v>116.9542</v>
       </c>
       <c r="O15">
-        <v>160.4941</v>
+        <v>135.05070000000001</v>
       </c>
       <c r="P15">
-        <v>174.2218</v>
+        <v>156.61760000000001</v>
       </c>
       <c r="Q15">
-        <v>188.1876</v>
+        <v>179.20570000000001</v>
       </c>
       <c r="R15">
-        <v>201.15880000000001</v>
+        <v>199.53200000000001</v>
       </c>
       <c r="S15">
-        <v>212.0737</v>
+        <v>214.35290000000001</v>
       </c>
       <c r="T15">
-        <v>220.23650000000001</v>
+        <v>221.49420000000001</v>
       </c>
       <c r="U15">
-        <v>225.39660000000001</v>
+        <v>220.4562</v>
       </c>
       <c r="V15">
-        <v>227.70179999999999</v>
+        <v>212.3066</v>
       </c>
       <c r="W15">
-        <v>227.57300000000001</v>
+        <v>199.05539999999999</v>
       </c>
       <c r="X15">
-        <v>225.55250000000001</v>
+        <v>182.87309999999999</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.2">
@@ -16107,70 +16119,70 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="D16">
-        <v>119.36360000000001</v>
+        <v>129.4948</v>
       </c>
       <c r="E16">
-        <v>118.12430000000001</v>
+        <v>129.8939</v>
       </c>
       <c r="F16">
-        <v>115.6494</v>
+        <v>130.73079999999999</v>
       </c>
       <c r="G16">
-        <v>112.1101</v>
+        <v>132.0889</v>
       </c>
       <c r="H16">
-        <v>106.51739999999999</v>
+        <v>131.43790000000001</v>
       </c>
       <c r="I16">
-        <v>98.261499999999998</v>
+        <v>127.6887</v>
       </c>
       <c r="J16">
-        <v>93.247200000000007</v>
+        <v>126.55800000000001</v>
       </c>
       <c r="K16">
-        <v>92.106499999999997</v>
+        <v>128.2311</v>
       </c>
       <c r="L16">
-        <v>95.413200000000003</v>
+        <v>132.9332</v>
       </c>
       <c r="M16">
-        <v>103.626</v>
+        <v>140.74029999999999</v>
       </c>
       <c r="N16">
-        <v>116.9542</v>
+        <v>151.43430000000001</v>
       </c>
       <c r="O16">
-        <v>135.05070000000001</v>
+        <v>164.4075</v>
       </c>
       <c r="P16">
-        <v>156.61760000000001</v>
+        <v>178.65440000000001</v>
       </c>
       <c r="Q16">
-        <v>179.20570000000001</v>
+        <v>192.89009999999999</v>
       </c>
       <c r="R16">
-        <v>199.53200000000001</v>
+        <v>205.78870000000001</v>
       </c>
       <c r="S16">
-        <v>214.35290000000001</v>
+        <v>216.26060000000001</v>
       </c>
       <c r="T16">
-        <v>221.49420000000001</v>
+        <v>223.65860000000001</v>
       </c>
       <c r="U16">
-        <v>220.4562</v>
+        <v>227.83709999999999</v>
       </c>
       <c r="V16">
-        <v>212.3066</v>
+        <v>229.07169999999999</v>
       </c>
       <c r="W16">
-        <v>199.05539999999999</v>
+        <v>227.899</v>
       </c>
       <c r="X16">
-        <v>182.87309999999999</v>
+        <v>224.94239999999999</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
@@ -16181,70 +16193,70 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="D17">
-        <v>129.4948</v>
+        <v>123.62390000000001</v>
       </c>
       <c r="E17">
-        <v>129.8939</v>
+        <v>124.3528</v>
       </c>
       <c r="F17">
-        <v>130.73079999999999</v>
+        <v>125.8903</v>
       </c>
       <c r="G17">
-        <v>132.0889</v>
+        <v>128.3433</v>
       </c>
       <c r="H17">
-        <v>131.43790000000001</v>
+        <v>128.8382</v>
       </c>
       <c r="I17">
-        <v>127.6887</v>
+        <v>126.5689</v>
       </c>
       <c r="J17">
-        <v>126.55800000000001</v>
+        <v>126.6358</v>
       </c>
       <c r="K17">
-        <v>128.2311</v>
+        <v>129.01249999999999</v>
       </c>
       <c r="L17">
-        <v>132.9332</v>
+        <v>133.75069999999999</v>
       </c>
       <c r="M17">
-        <v>140.74029999999999</v>
+        <v>140.82400000000001</v>
       </c>
       <c r="N17">
-        <v>151.43430000000001</v>
+        <v>150.02080000000001</v>
       </c>
       <c r="O17">
-        <v>164.4075</v>
+        <v>160.893</v>
       </c>
       <c r="P17">
-        <v>178.65440000000001</v>
+        <v>172.77350000000001</v>
       </c>
       <c r="Q17">
-        <v>192.89009999999999</v>
+        <v>184.86500000000001</v>
       </c>
       <c r="R17">
-        <v>205.78870000000001</v>
+        <v>196.3768</v>
       </c>
       <c r="S17">
-        <v>216.26060000000001</v>
+        <v>206.6635</v>
       </c>
       <c r="T17">
-        <v>223.65860000000001</v>
+        <v>215.31710000000001</v>
       </c>
       <c r="U17">
-        <v>227.83709999999999</v>
+        <v>222.1876</v>
       </c>
       <c r="V17">
-        <v>229.07169999999999</v>
+        <v>227.3426</v>
       </c>
       <c r="W17">
-        <v>227.899</v>
+        <v>230.99369999999999</v>
       </c>
       <c r="X17">
-        <v>224.94239999999999</v>
+        <v>233.42590000000001</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
@@ -16255,70 +16267,70 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="D18">
-        <v>123.62390000000001</v>
+        <v>102.11409999999999</v>
       </c>
       <c r="E18">
-        <v>124.3528</v>
+        <v>100.5271</v>
       </c>
       <c r="F18">
-        <v>125.8903</v>
+        <v>97.461200000000005</v>
       </c>
       <c r="G18">
-        <v>128.3433</v>
+        <v>93.177400000000006</v>
       </c>
       <c r="H18">
-        <v>128.8382</v>
+        <v>87.898799999999994</v>
       </c>
       <c r="I18">
-        <v>126.5689</v>
+        <v>79.667500000000004</v>
       </c>
       <c r="J18">
-        <v>126.6358</v>
+        <v>74.014099999999999</v>
       </c>
       <c r="K18">
-        <v>129.01249999999999</v>
+        <v>71.249300000000005</v>
       </c>
       <c r="L18">
-        <v>133.75069999999999</v>
+        <v>71.596900000000005</v>
       </c>
       <c r="M18">
-        <v>140.82400000000001</v>
+        <v>75.220299999999995</v>
       </c>
       <c r="N18">
-        <v>150.02080000000001</v>
+        <v>82.2286</v>
       </c>
       <c r="O18">
-        <v>160.893</v>
+        <v>92.606999999999999</v>
       </c>
       <c r="P18">
-        <v>172.77350000000001</v>
+        <v>106.0801</v>
       </c>
       <c r="Q18">
-        <v>184.86500000000001</v>
+        <v>121.97239999999999</v>
       </c>
       <c r="R18">
-        <v>196.3768</v>
+        <v>139.15950000000001</v>
       </c>
       <c r="S18">
-        <v>206.6635</v>
+        <v>156.18340000000001</v>
       </c>
       <c r="T18">
-        <v>215.31710000000001</v>
+        <v>171.5189</v>
       </c>
       <c r="U18">
-        <v>222.1876</v>
+        <v>183.8939</v>
       </c>
       <c r="V18">
-        <v>227.3426</v>
+        <v>192.53030000000001</v>
       </c>
       <c r="W18">
-        <v>230.99369999999999</v>
+        <v>197.22219999999999</v>
       </c>
       <c r="X18">
-        <v>233.42590000000001</v>
+        <v>198.2552</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
@@ -16329,70 +16341,70 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="D19">
-        <v>102.11409999999999</v>
+        <v>120.4198</v>
       </c>
       <c r="E19">
-        <v>100.5271</v>
+        <v>119.697</v>
       </c>
       <c r="F19">
-        <v>97.461200000000005</v>
+        <v>118.27</v>
       </c>
       <c r="G19">
-        <v>93.177400000000006</v>
+        <v>116.24890000000001</v>
       </c>
       <c r="H19">
-        <v>87.898799999999994</v>
+        <v>112.9515</v>
       </c>
       <c r="I19">
-        <v>79.667500000000004</v>
+        <v>105.95959999999999</v>
       </c>
       <c r="J19">
-        <v>74.014099999999999</v>
+        <v>101.6062</v>
       </c>
       <c r="K19">
-        <v>71.249300000000005</v>
+        <v>100.2689</v>
       </c>
       <c r="L19">
-        <v>71.596900000000005</v>
+        <v>102.2963</v>
       </c>
       <c r="M19">
-        <v>75.220299999999995</v>
+        <v>107.9173</v>
       </c>
       <c r="N19">
-        <v>82.2286</v>
+        <v>117.16330000000001</v>
       </c>
       <c r="O19">
-        <v>92.606999999999999</v>
+        <v>129.75980000000001</v>
       </c>
       <c r="P19">
-        <v>106.0801</v>
+        <v>145.00800000000001</v>
       </c>
       <c r="Q19">
-        <v>121.97239999999999</v>
+        <v>161.73769999999999</v>
       </c>
       <c r="R19">
-        <v>139.15950000000001</v>
+        <v>178.4128</v>
       </c>
       <c r="S19">
-        <v>156.18340000000001</v>
+        <v>193.40029999999999</v>
       </c>
       <c r="T19">
-        <v>171.5189</v>
+        <v>205.31559999999999</v>
       </c>
       <c r="U19">
-        <v>183.8939</v>
+        <v>213.2988</v>
       </c>
       <c r="V19">
-        <v>192.53030000000001</v>
+        <v>217.11750000000001</v>
       </c>
       <c r="W19">
-        <v>197.22219999999999</v>
+        <v>217.0898</v>
       </c>
       <c r="X19">
-        <v>198.2552</v>
+        <v>213.88140000000001</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
@@ -16403,70 +16415,70 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="D20">
-        <v>120.4198</v>
+        <v>104.9862</v>
       </c>
       <c r="E20">
-        <v>119.697</v>
+        <v>103.21980000000001</v>
       </c>
       <c r="F20">
-        <v>118.27</v>
+        <v>99.766800000000003</v>
       </c>
       <c r="G20">
-        <v>116.24890000000001</v>
+        <v>94.908100000000005</v>
       </c>
       <c r="H20">
-        <v>112.9515</v>
+        <v>88.516000000000005</v>
       </c>
       <c r="I20">
-        <v>105.95959999999999</v>
+        <v>79.714299999999994</v>
       </c>
       <c r="J20">
-        <v>101.6062</v>
+        <v>73.920100000000005</v>
       </c>
       <c r="K20">
-        <v>100.2689</v>
+        <v>71.619900000000001</v>
       </c>
       <c r="L20">
-        <v>102.2963</v>
+        <v>73.222499999999997</v>
       </c>
       <c r="M20">
-        <v>107.9173</v>
+        <v>79.109200000000001</v>
       </c>
       <c r="N20">
-        <v>117.16330000000001</v>
+        <v>89.6066</v>
       </c>
       <c r="O20">
-        <v>129.75980000000001</v>
+        <v>104.779</v>
       </c>
       <c r="P20">
-        <v>145.00800000000001</v>
+        <v>124.06019999999999</v>
       </c>
       <c r="Q20">
-        <v>161.73769999999999</v>
+        <v>145.90539999999999</v>
       </c>
       <c r="R20">
-        <v>178.4128</v>
+        <v>167.76179999999999</v>
       </c>
       <c r="S20">
-        <v>193.40029999999999</v>
+        <v>186.5615</v>
       </c>
       <c r="T20">
-        <v>205.31559999999999</v>
+        <v>199.60079999999999</v>
       </c>
       <c r="U20">
-        <v>213.2988</v>
+        <v>205.35069999999999</v>
       </c>
       <c r="V20">
-        <v>217.11750000000001</v>
+        <v>203.77539999999999</v>
       </c>
       <c r="W20">
-        <v>217.0898</v>
+        <v>196.06899999999999</v>
       </c>
       <c r="X20">
-        <v>213.88140000000001</v>
+        <v>184.0309</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
@@ -16477,70 +16489,70 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="D21">
-        <v>104.9862</v>
+        <v>107.2296</v>
       </c>
       <c r="E21">
-        <v>103.21980000000001</v>
+        <v>108.8289</v>
       </c>
       <c r="F21">
-        <v>99.766800000000003</v>
+        <v>112.24509999999999</v>
       </c>
       <c r="G21">
-        <v>94.908100000000005</v>
+        <v>117.7166</v>
       </c>
       <c r="H21">
-        <v>88.516000000000005</v>
+        <v>122.24209999999999</v>
       </c>
       <c r="I21">
-        <v>79.714299999999994</v>
+        <v>124.321</v>
       </c>
       <c r="J21">
-        <v>73.920100000000005</v>
+        <v>127.6748</v>
       </c>
       <c r="K21">
-        <v>71.619900000000001</v>
+        <v>131.2843</v>
       </c>
       <c r="L21">
-        <v>73.222499999999997</v>
+        <v>134.42609999999999</v>
       </c>
       <c r="M21">
-        <v>79.109200000000001</v>
+        <v>136.8665</v>
       </c>
       <c r="N21">
-        <v>89.6066</v>
+        <v>138.9212</v>
       </c>
       <c r="O21">
-        <v>104.779</v>
+        <v>141.32499999999999</v>
       </c>
       <c r="P21">
-        <v>124.06019999999999</v>
+        <v>144.9966</v>
       </c>
       <c r="Q21">
-        <v>145.90539999999999</v>
+        <v>150.83090000000001</v>
       </c>
       <c r="R21">
-        <v>167.76179999999999</v>
+        <v>159.58320000000001</v>
       </c>
       <c r="S21">
-        <v>186.5615</v>
+        <v>171.833</v>
       </c>
       <c r="T21">
-        <v>199.60079999999999</v>
+        <v>187.9838</v>
       </c>
       <c r="U21">
-        <v>205.35069999999999</v>
+        <v>208.26499999999999</v>
       </c>
       <c r="V21">
-        <v>203.77539999999999</v>
+        <v>232.72659999999999</v>
       </c>
       <c r="W21">
-        <v>196.06899999999999</v>
+        <v>261.23160000000001</v>
       </c>
       <c r="X21">
-        <v>184.0309</v>
+        <v>293.56049999999999</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
@@ -16551,70 +16563,70 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="D22">
-        <v>107.2296</v>
+        <v>127.1459</v>
       </c>
       <c r="E22">
-        <v>108.8289</v>
+        <v>126.9455</v>
       </c>
       <c r="F22">
-        <v>112.24509999999999</v>
+        <v>126.54519999999999</v>
       </c>
       <c r="G22">
-        <v>117.7166</v>
+        <v>126.0232</v>
       </c>
       <c r="H22">
-        <v>122.24209999999999</v>
+        <v>123.52760000000001</v>
       </c>
       <c r="I22">
-        <v>124.321</v>
+        <v>117.8519</v>
       </c>
       <c r="J22">
-        <v>127.6748</v>
+        <v>115.01600000000001</v>
       </c>
       <c r="K22">
-        <v>131.2843</v>
+        <v>115.4395</v>
       </c>
       <c r="L22">
-        <v>134.42609999999999</v>
+        <v>119.5347</v>
       </c>
       <c r="M22">
-        <v>136.8665</v>
+        <v>127.5342</v>
       </c>
       <c r="N22">
-        <v>138.9212</v>
+        <v>139.3313</v>
       </c>
       <c r="O22">
-        <v>141.32499999999999</v>
+        <v>154.31290000000001</v>
       </c>
       <c r="P22">
-        <v>144.9966</v>
+        <v>171.25049999999999</v>
       </c>
       <c r="Q22">
-        <v>150.83090000000001</v>
+        <v>188.3682</v>
       </c>
       <c r="R22">
-        <v>159.58320000000001</v>
+        <v>203.65459999999999</v>
       </c>
       <c r="S22">
-        <v>171.833</v>
+        <v>215.3373</v>
       </c>
       <c r="T22">
-        <v>187.9838</v>
+        <v>222.31100000000001</v>
       </c>
       <c r="U22">
-        <v>208.26499999999999</v>
+        <v>224.32259999999999</v>
       </c>
       <c r="V22">
-        <v>232.72659999999999</v>
+        <v>221.87270000000001</v>
       </c>
       <c r="W22">
-        <v>261.23160000000001</v>
+        <v>215.93020000000001</v>
       </c>
       <c r="X22">
-        <v>293.56049999999999</v>
+        <v>207.5924</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
@@ -16625,70 +16637,70 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="D23">
-        <v>127.1459</v>
+        <v>123.501</v>
       </c>
       <c r="E23">
-        <v>126.9455</v>
+        <v>122.46299999999999</v>
       </c>
       <c r="F23">
-        <v>126.54519999999999</v>
+        <v>120.3989</v>
       </c>
       <c r="G23">
-        <v>126.0232</v>
+        <v>117.45480000000001</v>
       </c>
       <c r="H23">
-        <v>123.52760000000001</v>
+        <v>112.7179</v>
       </c>
       <c r="I23">
-        <v>117.8519</v>
+        <v>104.776</v>
       </c>
       <c r="J23">
-        <v>115.01600000000001</v>
+        <v>99.891400000000004</v>
       </c>
       <c r="K23">
-        <v>115.4395</v>
+        <v>98.602400000000003</v>
       </c>
       <c r="L23">
-        <v>119.5347</v>
+        <v>101.39570000000001</v>
       </c>
       <c r="M23">
-        <v>127.5342</v>
+        <v>108.628</v>
       </c>
       <c r="N23">
-        <v>139.3313</v>
+        <v>120.4192</v>
       </c>
       <c r="O23">
-        <v>154.31290000000001</v>
+        <v>136.447</v>
       </c>
       <c r="P23">
-        <v>171.25049999999999</v>
+        <v>155.69710000000001</v>
       </c>
       <c r="Q23">
-        <v>188.3682</v>
+        <v>176.3415</v>
       </c>
       <c r="R23">
-        <v>203.65459999999999</v>
+        <v>195.93170000000001</v>
       </c>
       <c r="S23">
-        <v>215.3373</v>
+        <v>211.9409</v>
       </c>
       <c r="T23">
-        <v>222.31100000000001</v>
+        <v>222.43690000000001</v>
       </c>
       <c r="U23">
-        <v>224.32259999999999</v>
+        <v>226.55439999999999</v>
       </c>
       <c r="V23">
-        <v>221.87270000000001</v>
+        <v>224.5609</v>
       </c>
       <c r="W23">
-        <v>215.93020000000001</v>
+        <v>217.5608</v>
       </c>
       <c r="X23">
-        <v>207.5924</v>
+        <v>207.01320000000001</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
@@ -16699,70 +16711,70 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="D24">
-        <v>123.501</v>
+        <v>111.2907</v>
       </c>
       <c r="E24">
-        <v>122.46299999999999</v>
+        <v>109.8056</v>
       </c>
       <c r="F24">
-        <v>120.3989</v>
+        <v>106.8874</v>
       </c>
       <c r="G24">
-        <v>117.45480000000001</v>
+        <v>102.7556</v>
       </c>
       <c r="H24">
-        <v>112.7179</v>
+        <v>97.056700000000006</v>
       </c>
       <c r="I24">
-        <v>104.776</v>
+        <v>88.563100000000006</v>
       </c>
       <c r="J24">
-        <v>99.891400000000004</v>
+        <v>83.040099999999995</v>
       </c>
       <c r="K24">
-        <v>98.602400000000003</v>
+        <v>80.990499999999997</v>
       </c>
       <c r="L24">
-        <v>101.39570000000001</v>
+        <v>82.846000000000004</v>
       </c>
       <c r="M24">
-        <v>108.628</v>
+        <v>88.966899999999995</v>
       </c>
       <c r="N24">
-        <v>120.4192</v>
+        <v>99.589799999999997</v>
       </c>
       <c r="O24">
-        <v>136.447</v>
+        <v>114.6357</v>
       </c>
       <c r="P24">
-        <v>155.69710000000001</v>
+        <v>133.40700000000001</v>
       </c>
       <c r="Q24">
-        <v>176.3415</v>
+        <v>154.3441</v>
       </c>
       <c r="R24">
-        <v>195.93170000000001</v>
+        <v>175.07509999999999</v>
       </c>
       <c r="S24">
-        <v>211.9409</v>
+        <v>192.88300000000001</v>
       </c>
       <c r="T24">
-        <v>222.43690000000001</v>
+        <v>205.44290000000001</v>
       </c>
       <c r="U24">
-        <v>226.55439999999999</v>
+        <v>211.45590000000001</v>
       </c>
       <c r="V24">
-        <v>224.5609</v>
+        <v>210.87809999999999</v>
       </c>
       <c r="W24">
-        <v>217.5608</v>
+        <v>204.69499999999999</v>
       </c>
       <c r="X24">
-        <v>207.01320000000001</v>
+        <v>194.41569999999999</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
@@ -16773,70 +16785,70 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="D25">
-        <v>111.2907</v>
+        <v>103.8365</v>
       </c>
       <c r="E25">
-        <v>109.8056</v>
+        <v>101.91249999999999</v>
       </c>
       <c r="F25">
-        <v>106.8874</v>
+        <v>98.209599999999995</v>
       </c>
       <c r="G25">
-        <v>102.7556</v>
+        <v>93.054100000000005</v>
       </c>
       <c r="H25">
-        <v>97.056700000000006</v>
+        <v>86.770700000000005</v>
       </c>
       <c r="I25">
-        <v>88.563100000000006</v>
+        <v>77.719800000000006</v>
       </c>
       <c r="J25">
-        <v>83.040099999999995</v>
+        <v>71.498999999999995</v>
       </c>
       <c r="K25">
-        <v>80.990499999999997</v>
+        <v>68.481399999999994</v>
       </c>
       <c r="L25">
-        <v>82.846000000000004</v>
+        <v>68.947299999999998</v>
       </c>
       <c r="M25">
-        <v>88.966899999999995</v>
+        <v>73.145200000000003</v>
       </c>
       <c r="N25">
-        <v>99.589799999999997</v>
+        <v>81.308599999999998</v>
       </c>
       <c r="O25">
-        <v>114.6357</v>
+        <v>93.549000000000007</v>
       </c>
       <c r="P25">
-        <v>133.40700000000001</v>
+        <v>109.6296</v>
       </c>
       <c r="Q25">
-        <v>154.3441</v>
+        <v>128.7107</v>
       </c>
       <c r="R25">
-        <v>175.07509999999999</v>
+        <v>149.233</v>
       </c>
       <c r="S25">
-        <v>192.88300000000001</v>
+        <v>169.08539999999999</v>
       </c>
       <c r="T25">
-        <v>205.44290000000001</v>
+        <v>186.0598</v>
       </c>
       <c r="U25">
-        <v>211.45590000000001</v>
+        <v>198.40700000000001</v>
       </c>
       <c r="V25">
-        <v>210.87809999999999</v>
+        <v>205.22890000000001</v>
       </c>
       <c r="W25">
-        <v>204.69499999999999</v>
+        <v>206.5592</v>
       </c>
       <c r="X25">
-        <v>194.41569999999999</v>
+        <v>203.14449999999999</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
@@ -16847,70 +16859,70 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="D26">
-        <v>103.8365</v>
+        <v>102.8034</v>
       </c>
       <c r="E26">
-        <v>101.91249999999999</v>
+        <v>101.3604</v>
       </c>
       <c r="F26">
-        <v>98.209599999999995</v>
+        <v>98.461200000000005</v>
       </c>
       <c r="G26">
-        <v>93.054100000000005</v>
+        <v>94.302300000000002</v>
       </c>
       <c r="H26">
-        <v>86.770700000000005</v>
+        <v>87.9131</v>
       </c>
       <c r="I26">
-        <v>77.719800000000006</v>
+        <v>79.910899999999998</v>
       </c>
       <c r="J26">
-        <v>71.498999999999995</v>
+        <v>75.230099999999993</v>
       </c>
       <c r="K26">
-        <v>68.481399999999994</v>
+        <v>74.656800000000004</v>
       </c>
       <c r="L26">
-        <v>68.947299999999998</v>
+        <v>78.958799999999997</v>
       </c>
       <c r="M26">
-        <v>73.145200000000003</v>
+        <v>88.873800000000003</v>
       </c>
       <c r="N26">
-        <v>81.308599999999998</v>
+        <v>104.861</v>
       </c>
       <c r="O26">
-        <v>93.549000000000007</v>
+        <v>126.42659999999999</v>
       </c>
       <c r="P26">
-        <v>109.6296</v>
+        <v>151.2191</v>
       </c>
       <c r="Q26">
-        <v>128.7107</v>
+        <v>174.6815</v>
       </c>
       <c r="R26">
-        <v>149.233</v>
+        <v>191.1542</v>
       </c>
       <c r="S26">
-        <v>169.08539999999999</v>
+        <v>196.26669999999999</v>
       </c>
       <c r="T26">
-        <v>186.0598</v>
+        <v>188.994</v>
       </c>
       <c r="U26">
-        <v>198.40700000000001</v>
+        <v>171.80969999999999</v>
       </c>
       <c r="V26">
-        <v>205.22890000000001</v>
+        <v>149.05260000000001</v>
       </c>
       <c r="W26">
-        <v>206.5592</v>
+        <v>124.95350000000001</v>
       </c>
       <c r="X26">
-        <v>203.14449999999999</v>
+        <v>102.41289999999999</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
@@ -16921,70 +16933,70 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="D27">
-        <v>102.8034</v>
+        <v>109.1776</v>
       </c>
       <c r="E27">
-        <v>101.3604</v>
+        <v>107.5463</v>
       </c>
       <c r="F27">
-        <v>98.461200000000005</v>
+        <v>104.4435</v>
       </c>
       <c r="G27">
-        <v>94.302300000000002</v>
+        <v>100.1343</v>
       </c>
       <c r="H27">
-        <v>87.9131</v>
+        <v>95.289900000000003</v>
       </c>
       <c r="I27">
-        <v>79.910899999999998</v>
+        <v>86.613100000000003</v>
       </c>
       <c r="J27">
-        <v>75.230099999999993</v>
+        <v>80.429299999999998</v>
       </c>
       <c r="K27">
-        <v>74.656800000000004</v>
+        <v>77.009600000000006</v>
       </c>
       <c r="L27">
-        <v>78.958799999999997</v>
+        <v>76.545199999999994</v>
       </c>
       <c r="M27">
-        <v>88.873800000000003</v>
+        <v>79.156999999999996</v>
       </c>
       <c r="N27">
-        <v>104.861</v>
+        <v>84.907899999999998</v>
       </c>
       <c r="O27">
-        <v>126.42659999999999</v>
+        <v>93.767499999999998</v>
       </c>
       <c r="P27">
-        <v>151.2191</v>
+        <v>105.5288</v>
       </c>
       <c r="Q27">
-        <v>174.6815</v>
+        <v>119.71429999999999</v>
       </c>
       <c r="R27">
-        <v>191.1542</v>
+        <v>135.5316</v>
       </c>
       <c r="S27">
-        <v>196.26669999999999</v>
+        <v>151.92400000000001</v>
       </c>
       <c r="T27">
-        <v>188.994</v>
+        <v>167.72190000000001</v>
       </c>
       <c r="U27">
-        <v>171.80969999999999</v>
+        <v>181.845</v>
       </c>
       <c r="V27">
-        <v>149.05260000000001</v>
+        <v>193.48439999999999</v>
       </c>
       <c r="W27">
-        <v>124.95350000000001</v>
+        <v>202.19990000000001</v>
       </c>
       <c r="X27">
-        <v>102.41289999999999</v>
+        <v>207.93360000000001</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
@@ -16995,70 +17007,70 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="D28">
-        <v>109.1776</v>
+        <v>126.17059999999999</v>
       </c>
       <c r="E28">
-        <v>107.5463</v>
+        <v>126.87779999999999</v>
       </c>
       <c r="F28">
-        <v>104.4435</v>
+        <v>128.369</v>
       </c>
       <c r="G28">
-        <v>100.1343</v>
+        <v>130.7499</v>
       </c>
       <c r="H28">
-        <v>95.289900000000003</v>
+        <v>131.11869999999999</v>
       </c>
       <c r="I28">
-        <v>86.613100000000003</v>
+        <v>128.6634</v>
       </c>
       <c r="J28">
-        <v>80.429299999999998</v>
+        <v>128.61689999999999</v>
       </c>
       <c r="K28">
-        <v>77.009600000000006</v>
+        <v>130.9795</v>
       </c>
       <c r="L28">
-        <v>76.545199999999994</v>
+        <v>135.82570000000001</v>
       </c>
       <c r="M28">
-        <v>79.156999999999996</v>
+        <v>143.13910000000001</v>
       </c>
       <c r="N28">
-        <v>84.907899999999998</v>
+        <v>152.6985</v>
       </c>
       <c r="O28">
-        <v>93.767499999999998</v>
+        <v>164.02080000000001</v>
       </c>
       <c r="P28">
-        <v>105.5288</v>
+        <v>176.3784</v>
       </c>
       <c r="Q28">
-        <v>119.71429999999999</v>
+        <v>188.89709999999999</v>
       </c>
       <c r="R28">
-        <v>135.5316</v>
+        <v>200.7089</v>
       </c>
       <c r="S28">
-        <v>151.92400000000001</v>
+        <v>211.10980000000001</v>
       </c>
       <c r="T28">
-        <v>167.72190000000001</v>
+        <v>219.66380000000001</v>
       </c>
       <c r="U28">
-        <v>181.845</v>
+        <v>226.22620000000001</v>
       </c>
       <c r="V28">
-        <v>193.48439999999999</v>
+        <v>230.89590000000001</v>
       </c>
       <c r="W28">
-        <v>202.19990000000001</v>
+        <v>233.9297</v>
       </c>
       <c r="X28">
-        <v>207.93360000000001</v>
+        <v>235.65870000000001</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
@@ -17069,70 +17081,70 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="D29">
-        <v>126.17059999999999</v>
+        <v>133.08260000000001</v>
       </c>
       <c r="E29">
-        <v>126.87779999999999</v>
+        <v>133.5899</v>
       </c>
       <c r="F29">
-        <v>128.369</v>
+        <v>134.65979999999999</v>
       </c>
       <c r="G29">
-        <v>130.7499</v>
+        <v>136.3896</v>
       </c>
       <c r="H29">
-        <v>131.11869999999999</v>
+        <v>135.83279999999999</v>
       </c>
       <c r="I29">
-        <v>128.6634</v>
+        <v>132.37610000000001</v>
       </c>
       <c r="J29">
-        <v>128.61689999999999</v>
+        <v>131.64689999999999</v>
       </c>
       <c r="K29">
-        <v>130.9795</v>
+        <v>133.82230000000001</v>
       </c>
       <c r="L29">
-        <v>135.82570000000001</v>
+        <v>139.12270000000001</v>
       </c>
       <c r="M29">
-        <v>143.13910000000001</v>
+        <v>147.60650000000001</v>
       </c>
       <c r="N29">
-        <v>152.6985</v>
+        <v>159.011</v>
       </c>
       <c r="O29">
-        <v>164.02080000000001</v>
+        <v>172.654</v>
       </c>
       <c r="P29">
-        <v>176.3784</v>
+        <v>187.4385</v>
       </c>
       <c r="Q29">
-        <v>188.89709999999999</v>
+        <v>201.9999</v>
       </c>
       <c r="R29">
-        <v>200.7089</v>
+        <v>214.97620000000001</v>
       </c>
       <c r="S29">
-        <v>211.10980000000001</v>
+        <v>225.3022</v>
       </c>
       <c r="T29">
-        <v>219.66380000000001</v>
+        <v>232.40610000000001</v>
       </c>
       <c r="U29">
-        <v>226.22620000000001</v>
+        <v>236.2413</v>
       </c>
       <c r="V29">
-        <v>230.89590000000001</v>
+        <v>237.17500000000001</v>
       </c>
       <c r="W29">
-        <v>233.9297</v>
+        <v>235.80779999999999</v>
       </c>
       <c r="X29">
-        <v>235.65870000000001</v>
+        <v>232.79310000000001</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
@@ -17143,70 +17155,70 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="D30">
-        <v>133.08260000000001</v>
+        <v>132.54140000000001</v>
       </c>
       <c r="E30">
-        <v>133.5899</v>
+        <v>133.40799999999999</v>
       </c>
       <c r="F30">
-        <v>134.65979999999999</v>
+        <v>135.2364</v>
       </c>
       <c r="G30">
-        <v>136.3896</v>
+        <v>138.14769999999999</v>
       </c>
       <c r="H30">
-        <v>135.83279999999999</v>
+        <v>139.02959999999999</v>
       </c>
       <c r="I30">
-        <v>132.37610000000001</v>
+        <v>136.91550000000001</v>
       </c>
       <c r="J30">
-        <v>131.64689999999999</v>
+        <v>137.23699999999999</v>
       </c>
       <c r="K30">
-        <v>133.82230000000001</v>
+        <v>139.8963</v>
       </c>
       <c r="L30">
-        <v>139.12270000000001</v>
+        <v>144.893</v>
       </c>
       <c r="M30">
-        <v>147.60650000000001</v>
+        <v>152.17339999999999</v>
       </c>
       <c r="N30">
-        <v>159.011</v>
+        <v>161.529</v>
       </c>
       <c r="O30">
-        <v>172.654</v>
+        <v>172.5514</v>
       </c>
       <c r="P30">
-        <v>187.4385</v>
+        <v>184.649</v>
       </c>
       <c r="Q30">
-        <v>201.9999</v>
+        <v>197.12200000000001</v>
       </c>
       <c r="R30">
-        <v>214.97620000000001</v>
+        <v>209.2749</v>
       </c>
       <c r="S30">
-        <v>225.3022</v>
+        <v>220.5273</v>
       </c>
       <c r="T30">
-        <v>232.40610000000001</v>
+        <v>230.488</v>
       </c>
       <c r="U30">
-        <v>236.2413</v>
+        <v>238.97450000000001</v>
       </c>
       <c r="V30">
-        <v>237.17500000000001</v>
+        <v>245.98589999999999</v>
       </c>
       <c r="W30">
-        <v>235.80779999999999</v>
+        <v>251.64779999999999</v>
       </c>
       <c r="X30">
-        <v>232.79310000000001</v>
+        <v>256.16590000000002</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
@@ -17217,70 +17229,70 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="D31">
-        <v>132.54140000000001</v>
+        <v>129.05199999999999</v>
       </c>
       <c r="E31">
-        <v>133.40799999999999</v>
+        <v>129.52520000000001</v>
       </c>
       <c r="F31">
-        <v>135.2364</v>
+        <v>130.52180000000001</v>
       </c>
       <c r="G31">
-        <v>138.14769999999999</v>
+        <v>132.1328</v>
       </c>
       <c r="H31">
-        <v>139.02959999999999</v>
+        <v>131.59049999999999</v>
       </c>
       <c r="I31">
-        <v>136.91550000000001</v>
+        <v>128.15719999999999</v>
       </c>
       <c r="J31">
-        <v>137.23699999999999</v>
+        <v>127.35380000000001</v>
       </c>
       <c r="K31">
-        <v>139.8963</v>
+        <v>129.3511</v>
       </c>
       <c r="L31">
-        <v>144.893</v>
+        <v>134.36259999999999</v>
       </c>
       <c r="M31">
-        <v>152.17339999999999</v>
+        <v>142.4479</v>
       </c>
       <c r="N31">
-        <v>161.529</v>
+        <v>153.36320000000001</v>
       </c>
       <c r="O31">
-        <v>172.5514</v>
+        <v>166.4657</v>
       </c>
       <c r="P31">
-        <v>184.649</v>
+        <v>180.71629999999999</v>
       </c>
       <c r="Q31">
-        <v>197.12200000000001</v>
+        <v>194.8141</v>
       </c>
       <c r="R31">
-        <v>209.2749</v>
+        <v>207.44890000000001</v>
       </c>
       <c r="S31">
-        <v>220.5273</v>
+        <v>217.58109999999999</v>
       </c>
       <c r="T31">
-        <v>230.488</v>
+        <v>224.63380000000001</v>
       </c>
       <c r="U31">
-        <v>238.97450000000001</v>
+        <v>228.53200000000001</v>
       </c>
       <c r="V31">
-        <v>245.98589999999999</v>
+        <v>229.60249999999999</v>
       </c>
       <c r="W31">
-        <v>251.64779999999999</v>
+        <v>228.4074</v>
       </c>
       <c r="X31">
-        <v>256.16590000000002</v>
+        <v>225.56970000000001</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
@@ -17291,70 +17303,70 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="D32">
-        <v>129.05199999999999</v>
+        <v>133.3321</v>
       </c>
       <c r="E32">
-        <v>129.52520000000001</v>
+        <v>133.5163</v>
       </c>
       <c r="F32">
-        <v>130.52180000000001</v>
+        <v>133.90430000000001</v>
       </c>
       <c r="G32">
-        <v>132.1328</v>
+        <v>134.57259999999999</v>
       </c>
       <c r="H32">
-        <v>131.59049999999999</v>
+        <v>133.2901</v>
       </c>
       <c r="I32">
-        <v>128.15719999999999</v>
+        <v>128.6157</v>
       </c>
       <c r="J32">
-        <v>127.35380000000001</v>
+        <v>126.6957</v>
       </c>
       <c r="K32">
-        <v>129.3511</v>
+        <v>127.8039</v>
       </c>
       <c r="L32">
-        <v>134.36259999999999</v>
+        <v>132.2388</v>
       </c>
       <c r="M32">
-        <v>142.4479</v>
+        <v>140.13509999999999</v>
       </c>
       <c r="N32">
-        <v>153.36320000000001</v>
+        <v>151.3125</v>
       </c>
       <c r="O32">
-        <v>166.4657</v>
+        <v>165.15989999999999</v>
       </c>
       <c r="P32">
-        <v>180.71629999999999</v>
+        <v>180.5967</v>
       </c>
       <c r="Q32">
-        <v>194.8141</v>
+        <v>196.17420000000001</v>
       </c>
       <c r="R32">
-        <v>207.44890000000001</v>
+        <v>210.33269999999999</v>
       </c>
       <c r="S32">
-        <v>217.58109999999999</v>
+        <v>221.73509999999999</v>
       </c>
       <c r="T32">
-        <v>224.63380000000001</v>
+        <v>229.5403</v>
       </c>
       <c r="U32">
-        <v>228.53200000000001</v>
+        <v>233.51179999999999</v>
       </c>
       <c r="V32">
-        <v>229.60249999999999</v>
+        <v>233.94239999999999</v>
       </c>
       <c r="W32">
-        <v>228.4074</v>
+        <v>231.46960000000001</v>
       </c>
       <c r="X32">
-        <v>225.56970000000001</v>
+        <v>226.85390000000001</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
@@ -17365,70 +17377,70 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="D33">
-        <v>133.3321</v>
+        <v>103.61969999999999</v>
       </c>
       <c r="E33">
-        <v>133.5163</v>
+        <v>101.8753</v>
       </c>
       <c r="F33">
-        <v>133.90430000000001</v>
+        <v>98.437899999999999</v>
       </c>
       <c r="G33">
-        <v>134.57259999999999</v>
+        <v>93.580500000000001</v>
       </c>
       <c r="H33">
-        <v>133.2901</v>
+        <v>86.961399999999998</v>
       </c>
       <c r="I33">
-        <v>128.6157</v>
+        <v>78.277100000000004</v>
       </c>
       <c r="J33">
-        <v>126.6957</v>
+        <v>72.7226</v>
       </c>
       <c r="K33">
-        <v>127.8039</v>
+        <v>70.853300000000004</v>
       </c>
       <c r="L33">
-        <v>132.2388</v>
+        <v>73.158600000000007</v>
       </c>
       <c r="M33">
-        <v>140.13509999999999</v>
+        <v>80.116</v>
       </c>
       <c r="N33">
-        <v>151.3125</v>
+        <v>92.1297</v>
       </c>
       <c r="O33">
-        <v>165.15989999999999</v>
+        <v>109.2264</v>
       </c>
       <c r="P33">
-        <v>180.5967</v>
+        <v>130.5461</v>
       </c>
       <c r="Q33">
-        <v>196.17420000000001</v>
+        <v>153.91159999999999</v>
       </c>
       <c r="R33">
-        <v>210.33269999999999</v>
+        <v>175.9188</v>
       </c>
       <c r="S33">
-        <v>221.73509999999999</v>
+        <v>192.79060000000001</v>
       </c>
       <c r="T33">
-        <v>229.5403</v>
+        <v>201.66120000000001</v>
       </c>
       <c r="U33">
-        <v>233.51179999999999</v>
+        <v>201.5307</v>
       </c>
       <c r="V33">
-        <v>233.94239999999999</v>
+        <v>193.35730000000001</v>
       </c>
       <c r="W33">
-        <v>231.46960000000001</v>
+        <v>179.3776</v>
       </c>
       <c r="X33">
-        <v>226.85390000000001</v>
+        <v>162.13130000000001</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
@@ -17439,70 +17451,70 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D34">
-        <v>103.61969999999999</v>
+        <v>126.1455</v>
       </c>
       <c r="E34">
-        <v>101.8753</v>
+        <v>125.4808</v>
       </c>
       <c r="F34">
-        <v>98.437899999999999</v>
+        <v>124.1448</v>
       </c>
       <c r="G34">
-        <v>93.580500000000001</v>
+        <v>122.24339999999999</v>
       </c>
       <c r="H34">
-        <v>86.961399999999998</v>
+        <v>118.321</v>
       </c>
       <c r="I34">
-        <v>78.277100000000004</v>
+        <v>111.29989999999999</v>
       </c>
       <c r="J34">
-        <v>72.7226</v>
+        <v>107.32980000000001</v>
       </c>
       <c r="K34">
-        <v>70.853300000000004</v>
+        <v>106.9545</v>
       </c>
       <c r="L34">
-        <v>73.158600000000007</v>
+        <v>110.6833</v>
       </c>
       <c r="M34">
-        <v>80.116</v>
+        <v>118.85590000000001</v>
       </c>
       <c r="N34">
-        <v>92.1297</v>
+        <v>131.4879</v>
       </c>
       <c r="O34">
-        <v>109.2264</v>
+        <v>148.04499999999999</v>
       </c>
       <c r="P34">
-        <v>130.5461</v>
+        <v>167.22630000000001</v>
       </c>
       <c r="Q34">
-        <v>153.91159999999999</v>
+        <v>186.94229999999999</v>
       </c>
       <c r="R34">
-        <v>175.9188</v>
+        <v>204.64439999999999</v>
       </c>
       <c r="S34">
-        <v>192.79060000000001</v>
+        <v>217.95769999999999</v>
       </c>
       <c r="T34">
-        <v>201.66120000000001</v>
+        <v>225.3289</v>
       </c>
       <c r="U34">
-        <v>201.5307</v>
+        <v>226.36619999999999</v>
       </c>
       <c r="V34">
-        <v>193.35730000000001</v>
+        <v>221.74359999999999</v>
       </c>
       <c r="W34">
-        <v>179.3776</v>
+        <v>212.80459999999999</v>
       </c>
       <c r="X34">
-        <v>162.13130000000001</v>
+        <v>201.0616</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
@@ -17513,7 +17525,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D35">
         <v>126.1455</v>
@@ -17587,7 +17599,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D36">
         <v>126.1455</v>
@@ -17661,7 +17673,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D37">
         <v>126.1455</v>
@@ -17735,7 +17747,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D38">
         <v>126.1455</v>
@@ -17809,7 +17821,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D39">
         <v>126.1455</v>
@@ -17883,7 +17895,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D40">
         <v>126.1455</v>
@@ -17957,7 +17969,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D41">
         <v>126.1455</v>
@@ -18020,80 +18032,6 @@
         <v>212.80459999999999</v>
       </c>
       <c r="X41">
-        <v>201.0616</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42">
-        <v>2019</v>
-      </c>
-      <c r="D42">
-        <v>126.1455</v>
-      </c>
-      <c r="E42">
-        <v>125.4808</v>
-      </c>
-      <c r="F42">
-        <v>124.1448</v>
-      </c>
-      <c r="G42">
-        <v>122.24339999999999</v>
-      </c>
-      <c r="H42">
-        <v>118.321</v>
-      </c>
-      <c r="I42">
-        <v>111.29989999999999</v>
-      </c>
-      <c r="J42">
-        <v>107.32980000000001</v>
-      </c>
-      <c r="K42">
-        <v>106.9545</v>
-      </c>
-      <c r="L42">
-        <v>110.6833</v>
-      </c>
-      <c r="M42">
-        <v>118.85590000000001</v>
-      </c>
-      <c r="N42">
-        <v>131.4879</v>
-      </c>
-      <c r="O42">
-        <v>148.04499999999999</v>
-      </c>
-      <c r="P42">
-        <v>167.22630000000001</v>
-      </c>
-      <c r="Q42">
-        <v>186.94229999999999</v>
-      </c>
-      <c r="R42">
-        <v>204.64439999999999</v>
-      </c>
-      <c r="S42">
-        <v>217.95769999999999</v>
-      </c>
-      <c r="T42">
-        <v>225.3289</v>
-      </c>
-      <c r="U42">
-        <v>226.36619999999999</v>
-      </c>
-      <c r="V42">
-        <v>221.74359999999999</v>
-      </c>
-      <c r="W42">
-        <v>212.80459999999999</v>
-      </c>
-      <c r="X42">
         <v>201.0616</v>
       </c>
     </row>
@@ -18106,8 +18044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView zoomScale="175" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18276,7 +18214,7 @@
         <v>85</v>
       </c>
       <c r="B21" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -29936,8 +29874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:I401"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="R142" sqref="R142"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated TMB, re-ran all models to see what's working & whats not
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_220401.xlsx
+++ b/data/hake_intrasp_220401.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F2ADC9-9B15-D641-9D89-743FA69C9714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631C6728-0F2A-3540-AAC9-74101219EFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="33340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="503">
   <si>
     <t>Number</t>
   </si>
@@ -1524,12 +1524,6 @@
     <t>BTempC</t>
   </si>
   <si>
-    <t>...25</t>
-  </si>
-  <si>
-    <t>...26</t>
-  </si>
-  <si>
     <t>Pred</t>
   </si>
   <si>
@@ -4513,7 +4507,7 @@
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4590,7 +4584,7 @@
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4667,7 +4661,7 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4744,7 +4738,7 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -4821,7 +4815,7 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4898,7 +4892,7 @@
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4975,7 +4969,7 @@
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5052,7 +5046,7 @@
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5129,7 +5123,7 @@
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5206,7 +5200,7 @@
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5283,7 +5277,7 @@
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5360,7 +5354,7 @@
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -5437,7 +5431,7 @@
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -5514,7 +5508,7 @@
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -5591,7 +5585,7 @@
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -5668,7 +5662,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -5745,7 +5739,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -5822,7 +5816,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -5899,7 +5893,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -5976,7 +5970,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -6053,7 +6047,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -6130,7 +6124,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -6207,7 +6201,7 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -6284,7 +6278,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -6361,7 +6355,7 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -6438,7 +6432,7 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -6515,7 +6509,7 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -6592,7 +6586,7 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -6669,7 +6663,7 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -6746,7 +6740,7 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -6823,7 +6817,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -6900,7 +6894,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -6977,7 +6971,7 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -7054,7 +7048,7 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -7131,7 +7125,7 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -7208,7 +7202,7 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -7285,7 +7279,7 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -7362,7 +7356,7 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -7439,7 +7433,7 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -7516,7 +7510,7 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -7593,7 +7587,7 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -7670,7 +7664,7 @@
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -7747,7 +7741,7 @@
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -7824,7 +7818,7 @@
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -7901,7 +7895,7 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -7978,7 +7972,7 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -8055,7 +8049,7 @@
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -8132,7 +8126,7 @@
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -8209,7 +8203,7 @@
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -8286,7 +8280,7 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -8363,7 +8357,7 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B52">
         <v>2</v>
@@ -8440,7 +8434,7 @@
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -8517,7 +8511,7 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -8594,7 +8588,7 @@
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -8671,7 +8665,7 @@
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B56">
         <v>2</v>
@@ -8748,7 +8742,7 @@
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -8825,7 +8819,7 @@
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -8902,7 +8896,7 @@
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -8979,7 +8973,7 @@
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B60">
         <v>2</v>
@@ -9056,7 +9050,7 @@
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -9133,7 +9127,7 @@
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B62">
         <v>2</v>
@@ -9210,7 +9204,7 @@
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B63">
         <v>2</v>
@@ -9287,7 +9281,7 @@
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B64">
         <v>2</v>
@@ -9364,7 +9358,7 @@
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B65">
         <v>2</v>
@@ -9441,7 +9435,7 @@
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B66">
         <v>2</v>
@@ -9518,7 +9512,7 @@
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B67">
         <v>2</v>
@@ -9595,7 +9589,7 @@
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -9672,7 +9666,7 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B69">
         <v>2</v>
@@ -9749,7 +9743,7 @@
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B70">
         <v>2</v>
@@ -9826,7 +9820,7 @@
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B71">
         <v>2</v>
@@ -9903,7 +9897,7 @@
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B72">
         <v>2</v>
@@ -9980,7 +9974,7 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B73">
         <v>2</v>
@@ -10057,7 +10051,7 @@
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B74">
         <v>2</v>
@@ -10134,7 +10128,7 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B75">
         <v>2</v>
@@ -10211,7 +10205,7 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B76">
         <v>2</v>
@@ -10288,7 +10282,7 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B77">
         <v>2</v>
@@ -10365,7 +10359,7 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B78">
         <v>2</v>
@@ -10442,7 +10436,7 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B79">
         <v>2</v>
@@ -10519,7 +10513,7 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B80">
         <v>2</v>
@@ -10596,7 +10590,7 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -10673,7 +10667,7 @@
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B82">
         <v>3</v>
@@ -10750,7 +10744,7 @@
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B83">
         <v>3</v>
@@ -10827,7 +10821,7 @@
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B84">
         <v>3</v>
@@ -10904,7 +10898,7 @@
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B85">
         <v>3</v>
@@ -10981,7 +10975,7 @@
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B86">
         <v>3</v>
@@ -11058,7 +11052,7 @@
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B87">
         <v>3</v>
@@ -11135,7 +11129,7 @@
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B88">
         <v>3</v>
@@ -11212,7 +11206,7 @@
     </row>
     <row r="89" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B89">
         <v>3</v>
@@ -11289,7 +11283,7 @@
     </row>
     <row r="90" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B90">
         <v>3</v>
@@ -11366,7 +11360,7 @@
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B91">
         <v>3</v>
@@ -11443,7 +11437,7 @@
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B92">
         <v>3</v>
@@ -11520,7 +11514,7 @@
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B93">
         <v>3</v>
@@ -11597,7 +11591,7 @@
     </row>
     <row r="94" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B94">
         <v>3</v>
@@ -11674,7 +11668,7 @@
     </row>
     <row r="95" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B95">
         <v>3</v>
@@ -11751,7 +11745,7 @@
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B96">
         <v>3</v>
@@ -11828,7 +11822,7 @@
     </row>
     <row r="97" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B97">
         <v>3</v>
@@ -11905,7 +11899,7 @@
     </row>
     <row r="98" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B98">
         <v>3</v>
@@ -11982,7 +11976,7 @@
     </row>
     <row r="99" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B99">
         <v>3</v>
@@ -12059,7 +12053,7 @@
     </row>
     <row r="100" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B100">
         <v>3</v>
@@ -12136,7 +12130,7 @@
     </row>
     <row r="101" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B101">
         <v>3</v>
@@ -12213,7 +12207,7 @@
     </row>
     <row r="102" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B102">
         <v>3</v>
@@ -12290,7 +12284,7 @@
     </row>
     <row r="103" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B103">
         <v>3</v>
@@ -12367,7 +12361,7 @@
     </row>
     <row r="104" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B104">
         <v>3</v>
@@ -12444,7 +12438,7 @@
     </row>
     <row r="105" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B105">
         <v>3</v>
@@ -12521,7 +12515,7 @@
     </row>
     <row r="106" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B106">
         <v>3</v>
@@ -12598,7 +12592,7 @@
     </row>
     <row r="107" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B107">
         <v>3</v>
@@ -12675,7 +12669,7 @@
     </row>
     <row r="108" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B108">
         <v>3</v>
@@ -12752,7 +12746,7 @@
     </row>
     <row r="109" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B109">
         <v>3</v>
@@ -12829,7 +12823,7 @@
     </row>
     <row r="110" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B110">
         <v>3</v>
@@ -12906,7 +12900,7 @@
     </row>
     <row r="111" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B111">
         <v>3</v>
@@ -12983,7 +12977,7 @@
     </row>
     <row r="112" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B112">
         <v>3</v>
@@ -13060,7 +13054,7 @@
     </row>
     <row r="113" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B113">
         <v>3</v>
@@ -13137,7 +13131,7 @@
     </row>
     <row r="114" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B114">
         <v>3</v>
@@ -13214,7 +13208,7 @@
     </row>
     <row r="115" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B115">
         <v>3</v>
@@ -13291,7 +13285,7 @@
     </row>
     <row r="116" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B116">
         <v>3</v>
@@ -13368,7 +13362,7 @@
     </row>
     <row r="117" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B117">
         <v>3</v>
@@ -13445,7 +13439,7 @@
     </row>
     <row r="118" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B118">
         <v>3</v>
@@ -13522,7 +13516,7 @@
     </row>
     <row r="119" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B119">
         <v>3</v>
@@ -13599,7 +13593,7 @@
     </row>
     <row r="120" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B120">
         <v>3</v>
@@ -13676,7 +13670,7 @@
     </row>
     <row r="121" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B121">
         <v>3</v>
@@ -14506,8 +14500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14517,7 +14511,7 @@
         <v>163</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -14557,7 +14551,7 @@
         <v>144</v>
       </c>
       <c r="B6">
-        <v>8.3500000000000005E-2</v>
+        <v>0.16700000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -14565,7 +14559,7 @@
         <v>146</v>
       </c>
       <c r="B7">
-        <v>-0.46023779999999997</v>
+        <v>-0.46</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -14597,7 +14591,7 @@
         <v>152</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -14605,7 +14599,7 @@
         <v>153</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -14613,7 +14607,7 @@
         <v>154</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -14966,15 +14960,15 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:AG41"/>
+  <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D2" sqref="D2:W41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -15044,38 +15038,8 @@
       <c r="W1" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -15145,11 +15109,8 @@
       <c r="W2">
         <v>212.80459999999999</v>
       </c>
-      <c r="X2">
-        <v>201.0616</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -15219,11 +15180,8 @@
       <c r="W3">
         <v>152.9573</v>
       </c>
-      <c r="X3">
-        <v>130.83930000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -15293,11 +15251,8 @@
       <c r="W4">
         <v>302.23809999999997</v>
       </c>
-      <c r="X4">
-        <v>293.83179999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -15367,11 +15322,8 @@
       <c r="W5">
         <v>210.6893</v>
       </c>
-      <c r="X5">
-        <v>191.25540000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -15441,11 +15393,8 @@
       <c r="W6">
         <v>161.19159999999999</v>
       </c>
-      <c r="X6">
-        <v>149.37389999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -15515,11 +15464,8 @@
       <c r="W7">
         <v>225.27979999999999</v>
       </c>
-      <c r="X7">
-        <v>208.79150000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -15589,11 +15535,8 @@
       <c r="W8">
         <v>246.62549999999999</v>
       </c>
-      <c r="X8">
-        <v>241.27199999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -15663,11 +15606,8 @@
       <c r="W9">
         <v>201.26410000000001</v>
       </c>
-      <c r="X9">
-        <v>195.29329999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -15737,11 +15677,8 @@
       <c r="W10">
         <v>202.52959999999999</v>
       </c>
-      <c r="X10">
-        <v>194.1514</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -15811,11 +15748,8 @@
       <c r="W11">
         <v>215.49170000000001</v>
       </c>
-      <c r="X11">
-        <v>199.44579999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -15885,11 +15819,8 @@
       <c r="W12">
         <v>213.1063</v>
       </c>
-      <c r="X12">
-        <v>205.34800000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -15959,11 +15890,8 @@
       <c r="W13">
         <v>205.61179999999999</v>
       </c>
-      <c r="X13">
-        <v>197.10740000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -16033,11 +15961,8 @@
       <c r="W14">
         <v>227.57300000000001</v>
       </c>
-      <c r="X14">
-        <v>225.55250000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -16107,11 +16032,8 @@
       <c r="W15">
         <v>199.05539999999999</v>
       </c>
-      <c r="X15">
-        <v>182.87309999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -16181,11 +16103,8 @@
       <c r="W16">
         <v>227.899</v>
       </c>
-      <c r="X16">
-        <v>224.94239999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -16255,11 +16174,8 @@
       <c r="W17">
         <v>230.99369999999999</v>
       </c>
-      <c r="X17">
-        <v>233.42590000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -16329,11 +16245,8 @@
       <c r="W18">
         <v>197.22219999999999</v>
       </c>
-      <c r="X18">
-        <v>198.2552</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -16403,11 +16316,8 @@
       <c r="W19">
         <v>217.0898</v>
       </c>
-      <c r="X19">
-        <v>213.88140000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -16477,11 +16387,8 @@
       <c r="W20">
         <v>196.06899999999999</v>
       </c>
-      <c r="X20">
-        <v>184.0309</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -16551,11 +16458,8 @@
       <c r="W21">
         <v>261.23160000000001</v>
       </c>
-      <c r="X21">
-        <v>293.56049999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -16625,11 +16529,8 @@
       <c r="W22">
         <v>215.93020000000001</v>
       </c>
-      <c r="X22">
-        <v>207.5924</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -16699,11 +16600,8 @@
       <c r="W23">
         <v>217.5608</v>
       </c>
-      <c r="X23">
-        <v>207.01320000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -16773,11 +16671,8 @@
       <c r="W24">
         <v>204.69499999999999</v>
       </c>
-      <c r="X24">
-        <v>194.41569999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -16847,11 +16742,8 @@
       <c r="W25">
         <v>206.5592</v>
       </c>
-      <c r="X25">
-        <v>203.14449999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -16921,11 +16813,8 @@
       <c r="W26">
         <v>124.95350000000001</v>
       </c>
-      <c r="X26">
-        <v>102.41289999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -16995,11 +16884,8 @@
       <c r="W27">
         <v>202.19990000000001</v>
       </c>
-      <c r="X27">
-        <v>207.93360000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -17069,11 +16955,8 @@
       <c r="W28">
         <v>233.9297</v>
       </c>
-      <c r="X28">
-        <v>235.65870000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -17143,11 +17026,8 @@
       <c r="W29">
         <v>235.80779999999999</v>
       </c>
-      <c r="X29">
-        <v>232.79310000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -17217,11 +17097,8 @@
       <c r="W30">
         <v>251.64779999999999</v>
       </c>
-      <c r="X30">
-        <v>256.16590000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -17291,11 +17168,8 @@
       <c r="W31">
         <v>228.4074</v>
       </c>
-      <c r="X31">
-        <v>225.56970000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -17365,11 +17239,8 @@
       <c r="W32">
         <v>231.46960000000001</v>
       </c>
-      <c r="X32">
-        <v>226.85390000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -17439,11 +17310,8 @@
       <c r="W33">
         <v>179.3776</v>
       </c>
-      <c r="X33">
-        <v>162.13130000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -17513,11 +17381,8 @@
       <c r="W34">
         <v>212.80459999999999</v>
       </c>
-      <c r="X34">
-        <v>201.0616</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -17587,11 +17452,8 @@
       <c r="W35">
         <v>212.80459999999999</v>
       </c>
-      <c r="X35">
-        <v>201.0616</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -17661,11 +17523,8 @@
       <c r="W36">
         <v>212.80459999999999</v>
       </c>
-      <c r="X36">
-        <v>201.0616</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -17735,11 +17594,8 @@
       <c r="W37">
         <v>212.80459999999999</v>
       </c>
-      <c r="X37">
-        <v>201.0616</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -17809,11 +17665,8 @@
       <c r="W38">
         <v>212.80459999999999</v>
       </c>
-      <c r="X38">
-        <v>201.0616</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -17883,11 +17736,8 @@
       <c r="W39">
         <v>212.80459999999999</v>
       </c>
-      <c r="X39">
-        <v>201.0616</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -17957,11 +17807,8 @@
       <c r="W40">
         <v>212.80459999999999</v>
       </c>
-      <c r="X40">
-        <v>201.0616</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -18030,9 +17877,6 @@
       </c>
       <c r="W41">
         <v>212.80459999999999</v>
-      </c>
-      <c r="X41">
-        <v>201.0616</v>
       </c>
     </row>
   </sheetData>
@@ -18044,7 +17888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+    <sheetView zoomScale="175" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -18059,7 +17903,7 @@
         <v>163</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -18238,22 +18082,22 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>496</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>167</v>
@@ -18262,7 +18106,7 @@
         <v>175</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -29886,22 +29730,22 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>496</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>167</v>
@@ -29910,7 +29754,7 @@
         <v>175</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -41621,7 +41465,7 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -41674,7 +41518,7 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -41791,7 +41635,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -41820,7 +41664,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -41849,7 +41693,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -41878,7 +41722,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -41907,7 +41751,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -41936,7 +41780,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -41965,7 +41809,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -41994,7 +41838,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -42023,7 +41867,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -42052,7 +41896,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -42081,7 +41925,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -42110,7 +41954,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -42139,7 +41983,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -42168,7 +42012,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -42197,7 +42041,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -42226,7 +42070,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -42255,7 +42099,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -42284,7 +42128,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -42313,7 +42157,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -42342,7 +42186,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -42371,7 +42215,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -42400,7 +42244,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -42429,7 +42273,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -42458,7 +42302,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -42487,7 +42331,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -42557,7 +42401,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -42583,7 +42427,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -42609,7 +42453,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -42635,7 +42479,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -42661,7 +42505,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -42687,7 +42531,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -42713,7 +42557,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -42739,7 +42583,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -42765,7 +42609,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -42791,7 +42635,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -42817,7 +42661,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -42843,7 +42687,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -42869,7 +42713,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -42895,7 +42739,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -42921,7 +42765,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -42947,7 +42791,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -42973,7 +42817,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -42999,7 +42843,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -43025,7 +42869,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -43051,7 +42895,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -43077,7 +42921,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -43103,7 +42947,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -43129,7 +42973,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -43155,7 +42999,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -43181,7 +43025,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -43207,7 +43051,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -43233,7 +43077,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -43259,7 +43103,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -43285,7 +43129,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -43311,7 +43155,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -43337,7 +43181,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -43363,7 +43207,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -43389,7 +43233,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -43415,7 +43259,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -43441,7 +43285,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -43467,7 +43311,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -43493,7 +43337,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -43519,7 +43363,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -43545,7 +43389,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -43571,7 +43415,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -43993,7 +43837,7 @@
     </row>
     <row r="2" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -44064,7 +43908,7 @@
     </row>
     <row r="3" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -44135,7 +43979,7 @@
     </row>
     <row r="4" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -44206,7 +44050,7 @@
     </row>
     <row r="5" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -44277,7 +44121,7 @@
     </row>
     <row r="6" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -44348,7 +44192,7 @@
     </row>
     <row r="7" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -44419,7 +44263,7 @@
     </row>
     <row r="8" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -44490,7 +44334,7 @@
     </row>
     <row r="9" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -44561,7 +44405,7 @@
     </row>
     <row r="10" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -44632,7 +44476,7 @@
     </row>
     <row r="11" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -44703,7 +44547,7 @@
     </row>
     <row r="12" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -44774,7 +44618,7 @@
     </row>
     <row r="13" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -44845,7 +44689,7 @@
     </row>
     <row r="14" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -44916,7 +44760,7 @@
     </row>
     <row r="15" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -44987,7 +44831,7 @@
     </row>
     <row r="16" spans="1:125" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -45058,7 +44902,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -45129,7 +44973,7 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -45200,7 +45044,7 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -45271,7 +45115,7 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -45342,7 +45186,7 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -45413,7 +45257,7 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -45484,7 +45328,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -45555,7 +45399,7 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -45626,7 +45470,7 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -45697,7 +45541,7 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -45768,7 +45612,7 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -45839,7 +45683,7 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -45910,7 +45754,7 @@
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -45981,7 +45825,7 @@
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -46052,7 +45896,7 @@
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -46123,7 +45967,7 @@
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -46194,7 +46038,7 @@
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -46265,7 +46109,7 @@
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -46336,7 +46180,7 @@
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -46407,7 +46251,7 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -46478,7 +46322,7 @@
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -46549,7 +46393,7 @@
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -46620,7 +46464,7 @@
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -46691,7 +46535,7 @@
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -46762,7 +46606,7 @@
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -46833,7 +46677,7 @@
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -46904,7 +46748,7 @@
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -46975,7 +46819,7 @@
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -47046,7 +46890,7 @@
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -47117,7 +46961,7 @@
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -47188,7 +47032,7 @@
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -47259,7 +47103,7 @@
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -47330,7 +47174,7 @@
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -47401,7 +47245,7 @@
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -47472,7 +47316,7 @@
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -47543,7 +47387,7 @@
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -47614,7 +47458,7 @@
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -47685,7 +47529,7 @@
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -47856,7 +47700,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -47933,7 +47777,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -48010,7 +47854,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -48087,7 +47931,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -48164,7 +48008,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -48241,7 +48085,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -48318,7 +48162,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -48395,7 +48239,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -48472,7 +48316,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -48549,7 +48393,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -48626,7 +48470,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -48703,7 +48547,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -48780,7 +48624,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -48857,7 +48701,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -48934,7 +48778,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -49011,7 +48855,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -49088,7 +48932,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -49165,7 +49009,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -49242,7 +49086,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -49319,7 +49163,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -49396,7 +49240,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -49473,7 +49317,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -49550,7 +49394,7 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -49627,7 +49471,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -49704,7 +49548,7 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -49781,7 +49625,7 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -49858,7 +49702,7 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -49935,7 +49779,7 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -50012,7 +49856,7 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -50089,7 +49933,7 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -50166,7 +50010,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -50243,7 +50087,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -50320,7 +50164,7 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -50397,7 +50241,7 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -50474,7 +50318,7 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -50551,7 +50395,7 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -50628,7 +50472,7 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -50705,7 +50549,7 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -50782,7 +50626,7 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -50859,7 +50703,7 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -50936,7 +50780,7 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -51013,7 +50857,7 @@
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -51090,7 +50934,7 @@
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -51167,7 +51011,7 @@
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -51244,7 +51088,7 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -51321,7 +51165,7 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -51398,7 +51242,7 @@
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -51475,7 +51319,7 @@
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -51552,7 +51396,7 @@
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -51629,7 +51473,7 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -51706,7 +51550,7 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -51783,7 +51627,7 @@
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -51860,7 +51704,7 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -51937,7 +51781,7 @@
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -52014,7 +51858,7 @@
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -52091,7 +51935,7 @@
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -52168,7 +52012,7 @@
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -52245,7 +52089,7 @@
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -52322,7 +52166,7 @@
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -52399,7 +52243,7 @@
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -52476,7 +52320,7 @@
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -52553,7 +52397,7 @@
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -52630,7 +52474,7 @@
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -52707,7 +52551,7 @@
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -52784,7 +52628,7 @@
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -52861,7 +52705,7 @@
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -52938,7 +52782,7 @@
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -53015,7 +52859,7 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -53092,7 +52936,7 @@
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -53169,7 +53013,7 @@
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -53246,7 +53090,7 @@
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -53323,7 +53167,7 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -53400,7 +53244,7 @@
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -53477,7 +53321,7 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -53554,7 +53398,7 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -53631,7 +53475,7 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -53708,7 +53552,7 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -53785,7 +53629,7 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -53862,7 +53706,7 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -53939,7 +53783,7 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -54108,7 +53952,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -54182,7 +54026,7 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -54256,7 +54100,7 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -54330,7 +54174,7 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -54404,7 +54248,7 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -54478,7 +54322,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -54552,7 +54396,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -54626,7 +54470,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -54700,7 +54544,7 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -54774,7 +54618,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -54848,7 +54692,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -54922,7 +54766,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -54996,7 +54840,7 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -55070,7 +54914,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -55144,7 +54988,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -55218,7 +55062,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -55292,7 +55136,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -55366,7 +55210,7 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -55440,7 +55284,7 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -55514,7 +55358,7 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -55588,7 +55432,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -55662,7 +55506,7 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -55736,7 +55580,7 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -55810,7 +55654,7 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -55884,7 +55728,7 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -55958,7 +55802,7 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -56032,7 +55876,7 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -56106,7 +55950,7 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -56180,7 +56024,7 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -56254,7 +56098,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -56328,7 +56172,7 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -56402,7 +56246,7 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -56476,7 +56320,7 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -56550,7 +56394,7 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -56624,7 +56468,7 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -56698,7 +56542,7 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -56772,7 +56616,7 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -56846,7 +56690,7 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -56920,7 +56764,7 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -56994,7 +56838,7 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -57451,7 +57295,7 @@
     </row>
     <row r="2" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -57819,7 +57663,7 @@
     </row>
     <row r="3" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -58187,7 +58031,7 @@
     </row>
     <row r="4" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -58555,7 +58399,7 @@
     </row>
     <row r="5" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -58923,7 +58767,7 @@
     </row>
     <row r="6" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -59291,7 +59135,7 @@
     </row>
     <row r="7" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -59659,7 +59503,7 @@
     </row>
     <row r="8" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -60027,7 +59871,7 @@
     </row>
     <row r="9" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -60395,7 +60239,7 @@
     </row>
     <row r="10" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -60763,7 +60607,7 @@
     </row>
     <row r="11" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -61131,7 +60975,7 @@
     </row>
     <row r="12" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -61226,7 +61070,7 @@
     </row>
     <row r="13" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -61321,7 +61165,7 @@
     </row>
     <row r="14" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -61416,7 +61260,7 @@
     </row>
     <row r="15" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -61511,7 +61355,7 @@
     </row>
     <row r="16" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -61606,7 +61450,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -61701,7 +61545,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -61796,7 +61640,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -61891,7 +61735,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -61986,7 +61830,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B21">
         <v>1</v>

</xml_diff>